<commit_message>
check for negative values in tables
</commit_message>
<xml_diff>
--- a/notebooks/test_results.xlsx
+++ b/notebooks/test_results.xlsx
@@ -11,8 +11,9 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_0" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_2" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_3" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_4" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_5" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_5" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_6" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_7" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -430,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,12 +481,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>table = acro.pivot_table(</t>
+          <t>safe_table = acro.crosstab(df.year, df.grant_type, values=negative, aggfunc="mean")</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>pass</t>
+          <t>review; negative values found</t>
         </is>
       </c>
     </row>
@@ -497,44 +498,61 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>results = acro.ols(y, x)</t>
+          <t>table = acro.pivot_table(</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>pass; dof=807.0 &gt;= 10</t>
+          <t>pass</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>output_4</t>
+          <t>output_5</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>results = acro.probit(y, x)</t>
+          <t>results = acro.ols(y, x)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>pass; dof=806.0 &gt;= 10</t>
+          <t>pass; dof=807.0 &gt;= 10</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>output_5</t>
+          <t>output_6</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>results = acro.probit(y, x)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>pass; dof=806.0 &gt;= 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>output_7</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>results = acro.logit(y, x)</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>pass; dof=806.0 &gt;= 10</t>
         </is>
@@ -893,6 +911,304 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Command</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>safe_table = acro.crosstab(df.year, df.grant_type, values=negative, aggfunc="mean")</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Summary</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>review; negative values found</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>R/G</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="D13" s="1" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="E13" s="1" t="inlineStr">
+        <is>
+          <t>R/G</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B14" t="n">
+        <v>9921906</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>8280032.5</v>
+      </c>
+      <c r="E14" t="n">
+        <v>11636000</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B15" t="n">
+        <v>8502246</v>
+      </c>
+      <c r="C15" t="n">
+        <v>123496.4453125</v>
+      </c>
+      <c r="D15" t="n">
+        <v>7577703.5</v>
+      </c>
+      <c r="E15" t="n">
+        <v>16047500</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B16" t="n">
+        <v>11458580</v>
+      </c>
+      <c r="C16" t="n">
+        <v>131859.0625</v>
+      </c>
+      <c r="D16" t="n">
+        <v>6796357.5</v>
+      </c>
+      <c r="E16" t="n">
+        <v>16810000</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B17" t="n">
+        <v>13557147</v>
+      </c>
+      <c r="C17" t="n">
+        <v>147937.625</v>
+      </c>
+      <c r="D17" t="n">
+        <v>6988263</v>
+      </c>
+      <c r="E17" t="n">
+        <v>16765625</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B18" t="n">
+        <v>13748147</v>
+      </c>
+      <c r="C18" t="n">
+        <v>133198.078125</v>
+      </c>
+      <c r="D18" t="n">
+        <v>7997392</v>
+      </c>
+      <c r="E18" t="n">
+        <v>17845750</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B19" t="n">
+        <v>11133433</v>
+      </c>
+      <c r="C19" t="n">
+        <v>146572.015625</v>
+      </c>
+      <c r="D19" t="n">
+        <v>10388612</v>
+      </c>
+      <c r="E19" t="n">
+        <v>18278624</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1121,7 +1437,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1203,7 +1519,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.894</v>
+        <v>0.893</v>
       </c>
     </row>
     <row r="7">
@@ -1223,7 +1539,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2276</v>
+        <v>2261</v>
       </c>
     </row>
     <row r="8">
@@ -1234,7 +1550,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Thu, 06 Oct 2022</t>
+          <t>Tue, 11 Oct 2022</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1254,7 +1570,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>15:22:23</t>
+          <t>20:21:17</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1263,7 +1579,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>-14493</v>
+        <v>-14495</v>
       </c>
     </row>
     <row r="10">
@@ -1283,7 +1599,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>28990</v>
+        <v>29000</v>
       </c>
     </row>
     <row r="11">
@@ -1303,7 +1619,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>29010</v>
+        <v>29020</v>
       </c>
     </row>
     <row r="12">
@@ -1373,22 +1689,22 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>399400</v>
+        <v>301000</v>
       </c>
       <c r="C16" t="n">
-        <v>531000</v>
+        <v>533000</v>
       </c>
       <c r="D16" t="n">
-        <v>0.752</v>
+        <v>0.5649999999999999</v>
       </c>
       <c r="E16" t="n">
-        <v>0.452</v>
+        <v>0.572</v>
       </c>
       <c r="F16" t="n">
-        <v>-643000</v>
+        <v>-745000</v>
       </c>
       <c r="G16" t="n">
-        <v>1440000</v>
+        <v>1350000</v>
       </c>
     </row>
     <row r="17">
@@ -1398,22 +1714,22 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.8856000000000001</v>
+        <v>-0.8846000000000001</v>
       </c>
       <c r="C17" t="n">
         <v>0.025</v>
       </c>
       <c r="D17" t="n">
-        <v>-36.128</v>
+        <v>-35.956</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.9340000000000001</v>
+        <v>-0.9330000000000001</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.837</v>
+        <v>-0.836</v>
       </c>
     </row>
     <row r="18">
@@ -1423,22 +1739,22 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.6659</v>
+        <v>-0.6647</v>
       </c>
       <c r="C18" t="n">
         <v>0.016</v>
       </c>
       <c r="D18" t="n">
-        <v>-40.905</v>
+        <v>-40.721</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.698</v>
+        <v>-0.697</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.634</v>
+        <v>-0.633</v>
       </c>
     </row>
     <row r="19">
@@ -1448,13 +1764,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.8318</v>
+        <v>0.8313</v>
       </c>
       <c r="C19" t="n">
         <v>0.011</v>
       </c>
       <c r="D19" t="n">
-        <v>78.937</v>
+        <v>78.67400000000001</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -1463,7 +1779,7 @@
         <v>0.8110000000000001</v>
       </c>
       <c r="G19" t="n">
-        <v>0.853</v>
+        <v>0.852</v>
       </c>
     </row>
     <row r="21">
@@ -1474,7 +1790,7 @@
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>1348.637</t>
+          <t>1339.956</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr">
@@ -1484,7 +1800,7 @@
       </c>
       <c r="D21" s="1" t="inlineStr">
         <is>
-          <t>1.424</t>
+          <t>1.414</t>
         </is>
       </c>
     </row>
@@ -1503,7 +1819,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>1298161.546</v>
+        <v>1253317.706</v>
       </c>
     </row>
     <row r="23">
@@ -1513,7 +1829,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>10.026</v>
+        <v>9.898999999999999</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1531,7 +1847,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>197.973</v>
+        <v>194.566</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1539,354 +1855,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>106000000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Command</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>results = acro.probit(y, x)</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Summary</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>pass; dof=806.0 &gt;= 10</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Dep. Variable:</t>
-        </is>
-      </c>
-      <c r="B5" s="1" t="inlineStr">
-        <is>
-          <t>survivor</t>
-        </is>
-      </c>
-      <c r="C5" s="1" t="inlineStr">
-        <is>
-          <t>No. Observations:</t>
-        </is>
-      </c>
-      <c r="D5" s="1" t="inlineStr">
-        <is>
-          <t>811</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Model:</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Probit</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Df Residuals:</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Method:</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>MLE</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Df Model:</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Date:</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Thu, 06 Oct 2022</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Pseudo R-squ.:</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>0.2086</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>Time:</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>15:22:23</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Log-Likelihood:</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>-403.24</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>converged:</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>LL-Null:</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>-509.5</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>Covariance Type:</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>nonrobust</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>LLR p-value:</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>7.648e-45</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" s="1" t="inlineStr">
-        <is>
-          <t>coef</t>
-        </is>
-      </c>
-      <c r="C13" s="1" t="inlineStr">
-        <is>
-          <t>std err</t>
-        </is>
-      </c>
-      <c r="D13" s="1" t="inlineStr">
-        <is>
-          <t>z</t>
-        </is>
-      </c>
-      <c r="E13" s="1" t="inlineStr">
-        <is>
-          <t>P&gt;|z|</t>
-        </is>
-      </c>
-      <c r="F13" s="1" t="inlineStr">
-        <is>
-          <t>[0.025</t>
-        </is>
-      </c>
-      <c r="G13" s="1" t="inlineStr">
-        <is>
-          <t>0.975]</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>const</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>0.0445</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.056</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.791</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.429</v>
-      </c>
-      <c r="F14" t="n">
-        <v>-0.066</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.155</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>inc_activity</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>4.114e-08</v>
-      </c>
-      <c r="C15" t="n">
-        <v>6.54e-08</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0.629</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="F15" t="n">
-        <v>-8.710000000000001e-08</v>
-      </c>
-      <c r="G15" t="n">
-        <v>1.69e-07</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>inc_grants</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>-4.297e-08</v>
-      </c>
-      <c r="C16" t="n">
-        <v>6.069999999999999e-08</v>
-      </c>
-      <c r="D16" t="n">
-        <v>-0.708</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.479</v>
-      </c>
-      <c r="F16" t="n">
-        <v>-1.62e-07</v>
-      </c>
-      <c r="G16" t="n">
-        <v>7.600000000000001e-08</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>inc_donations</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>1.357e-07</v>
-      </c>
-      <c r="C17" t="n">
-        <v>6.27e-08</v>
-      </c>
-      <c r="D17" t="n">
-        <v>2.163</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.031</v>
-      </c>
-      <c r="F17" t="n">
-        <v>1.28e-08</v>
-      </c>
-      <c r="G17" t="n">
-        <v>2.59e-07</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>total_costs</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>3.473e-08</v>
-      </c>
-      <c r="C18" t="n">
-        <v>5.84e-08</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0.595</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.552</v>
-      </c>
-      <c r="F18" t="n">
-        <v>-7.96e-08</v>
-      </c>
-      <c r="G18" t="n">
-        <v>1.49e-07</v>
+        <v>105000000</v>
       </c>
     </row>
   </sheetData>
@@ -1921,7 +1890,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>results = acro.logit(y, x)</t>
+          <t>results = acro.probit(y, x)</t>
         </is>
       </c>
     </row>
@@ -1967,7 +1936,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Logit</t>
+          <t>Probit</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2007,7 +1976,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Thu, 06 Oct 2022</t>
+          <t>Tue, 11 Oct 2022</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -2027,7 +1996,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>15:22:23</t>
+          <t>20:21:18</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -2076,7 +2045,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>4.862e-46</v>
+        <v>4.875e-46</v>
       </c>
     </row>
     <row r="13">
@@ -2118,22 +2087,369 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.0436</v>
+        <v>0.0474</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.057</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.838</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.402</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-0.063</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>inc_activity</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1.836e-07</v>
+      </c>
+      <c r="C15" t="n">
+        <v>5.16e-08</v>
+      </c>
+      <c r="D15" t="n">
+        <v>3.559</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>8.25e-08</v>
+      </c>
+      <c r="G15" t="n">
+        <v>2.85e-07</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>inc_grants</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>8.576e-08</v>
+      </c>
+      <c r="C16" t="n">
+        <v>3.9e-08</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2.197</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="F16" t="n">
+        <v>9.25e-09</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1.62e-07</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>inc_donations</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>2.406e-07</v>
+      </c>
+      <c r="C17" t="n">
+        <v>4.54e-08</v>
+      </c>
+      <c r="D17" t="n">
+        <v>5.297</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1.52e-07</v>
+      </c>
+      <c r="G17" t="n">
+        <v>3.3e-07</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>total_costs</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>-8.644e-08</v>
+      </c>
+      <c r="C18" t="n">
+        <v>3.68e-08</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-2.351</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-1.59e-07</v>
+      </c>
+      <c r="G18" t="n">
+        <v>-1.44e-08</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Command</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>results = acro.logit(y, x)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Summary</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>pass; dof=806.0 &gt;= 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Dep. Variable:</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>survivor</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>No. Observations:</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>811</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Model:</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Logit</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Df Residuals:</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Method:</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>MLE</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Df Model:</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Date:</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Tue, 11 Oct 2022</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Pseudo R-squ.:</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.2187</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Time:</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>20:21:18</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Log-Likelihood:</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>-398.07</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>converged:</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>LL-Null:</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>-509.5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Covariance Type:</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>nonrobust</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>LLR p-value:</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>4.532e-47</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>coef</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>std err</t>
+        </is>
+      </c>
+      <c r="D13" s="1" t="inlineStr">
+        <is>
+          <t>z</t>
+        </is>
+      </c>
+      <c r="E13" s="1" t="inlineStr">
+        <is>
+          <t>P&gt;|z|</t>
+        </is>
+      </c>
+      <c r="F13" s="1" t="inlineStr">
+        <is>
+          <t>[0.025</t>
+        </is>
+      </c>
+      <c r="G13" s="1" t="inlineStr">
+        <is>
+          <t>0.975]</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>const</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.0512</v>
       </c>
       <c r="C14" t="n">
         <v>0.091</v>
       </c>
       <c r="D14" t="n">
-        <v>0.48</v>
+        <v>0.5610000000000001</v>
       </c>
       <c r="E14" t="n">
-        <v>0.631</v>
+        <v>0.575</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.135</v>
+        <v>-0.128</v>
       </c>
       <c r="G14" t="n">
-        <v>0.222</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="15">
@@ -2143,22 +2459,22 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>5.79e-08</v>
+        <v>2.981e-07</v>
       </c>
       <c r="C15" t="n">
-        <v>1.13e-07</v>
+        <v>8.95e-08</v>
       </c>
       <c r="D15" t="n">
-        <v>0.513</v>
+        <v>3.33</v>
       </c>
       <c r="E15" t="n">
-        <v>0.608</v>
+        <v>0.001</v>
       </c>
       <c r="F15" t="n">
-        <v>-1.63e-07</v>
+        <v>1.23e-07</v>
       </c>
       <c r="G15" t="n">
-        <v>2.79e-07</v>
+        <v>4.74e-07</v>
       </c>
     </row>
     <row r="16">
@@ -2168,22 +2484,22 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-7.977000000000001e-08</v>
+        <v>1.351e-07</v>
       </c>
       <c r="C16" t="n">
-        <v>1.04e-07</v>
+        <v>6.67e-08</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.764</v>
+        <v>2.026</v>
       </c>
       <c r="E16" t="n">
-        <v>0.445</v>
+        <v>0.043</v>
       </c>
       <c r="F16" t="n">
-        <v>-2.85e-07</v>
+        <v>4.39e-09</v>
       </c>
       <c r="G16" t="n">
-        <v>1.25e-07</v>
+        <v>2.66e-07</v>
       </c>
     </row>
     <row r="17">
@@ -2193,22 +2509,22 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>3.638e-07</v>
+        <v>5.122999999999999e-07</v>
       </c>
       <c r="C17" t="n">
-        <v>1.31e-07</v>
+        <v>1.04e-07</v>
       </c>
       <c r="D17" t="n">
-        <v>2.772</v>
+        <v>4.927</v>
       </c>
       <c r="E17" t="n">
-        <v>0.006</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>1.07e-07</v>
+        <v>3.08e-07</v>
       </c>
       <c r="G17" t="n">
-        <v>6.21e-07</v>
+        <v>7.16e-07</v>
       </c>
     </row>
     <row r="18">
@@ -2218,22 +2534,22 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>5.649e-08</v>
+        <v>-1.442e-07</v>
       </c>
       <c r="C18" t="n">
-        <v>1e-07</v>
+        <v>6.26e-08</v>
       </c>
       <c r="D18" t="n">
-        <v>0.5639999999999999</v>
+        <v>-2.304</v>
       </c>
       <c r="E18" t="n">
-        <v>0.573</v>
+        <v>0.021</v>
       </c>
       <c r="F18" t="n">
-        <v>-1.4e-07</v>
+        <v>-2.67e-07</v>
       </c>
       <c r="G18" t="n">
-        <v>2.53e-07</v>
+        <v>-2.15e-08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set logging to info
</commit_message>
<xml_diff>
--- a/notebooks/test_results.xlsx
+++ b/notebooks/test_results.xlsx
@@ -1588,7 +1588,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>13:09:52</t>
+          <t>13:31:46</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -2014,7 +2014,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>13:09:52</t>
+          <t>13:31:47</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -2440,7 +2440,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>13:09:52</t>
+          <t>13:31:47</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -2787,7 +2787,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>13:09:52</t>
+          <t>13:31:47</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">

</xml_diff>

<commit_message>
seperating the analytic results out from json files
</commit_message>
<xml_diff>
--- a/notebooks/test_results.xlsx
+++ b/notebooks/test_results.xlsx
@@ -1136,7 +1136,7 @@
         <v>2011</v>
       </c>
       <c r="B15" t="n">
-        <v>8502246</v>
+        <v>8502247</v>
       </c>
       <c r="C15" t="n">
         <v>123496.4453125</v>
@@ -1176,7 +1176,7 @@
         <v>147937.625</v>
       </c>
       <c r="D17" t="n">
-        <v>6988263</v>
+        <v>6988263.5</v>
       </c>
       <c r="E17" t="n">
         <v>16765625</v>
@@ -1193,7 +1193,7 @@
         <v>133198.078125</v>
       </c>
       <c r="D18" t="n">
-        <v>7997392</v>
+        <v>7997392.5</v>
       </c>
       <c r="E18" t="n">
         <v>17845750</v>
@@ -1210,7 +1210,7 @@
         <v>146572.015625</v>
       </c>
       <c r="D19" t="n">
-        <v>10388612</v>
+        <v>10388613</v>
       </c>
       <c r="E19" t="n">
         <v>18278624</v>
@@ -1568,7 +1568,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Fri, 14 Oct 2022</t>
+          <t>Tue, 07 Mar 2023</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>15:38:52</t>
+          <t>10:45:02</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1994,7 +1994,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Fri, 14 Oct 2022</t>
+          <t>Tue, 07 Mar 2023</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -2014,7 +2014,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>15:38:52</t>
+          <t>10:45:02</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -2420,7 +2420,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Fri, 14 Oct 2022</t>
+          <t>Tue, 07 Mar 2023</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -2440,7 +2440,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>15:38:53</t>
+          <t>10:45:02</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -2767,7 +2767,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Fri, 14 Oct 2022</t>
+          <t>Tue, 07 Mar 2023</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -2787,7 +2787,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>15:38:53</t>
+          <t>10:45:02</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">

</xml_diff>

<commit_message>
changing the path of the output folder
</commit_message>
<xml_diff>
--- a/notebooks/test_results.xlsx
+++ b/notebooks/test_results.xlsx
@@ -1568,7 +1568,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Tue, 07 Mar 2023</t>
+          <t>Mon, 13 Mar 2023</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>10:45:02</t>
+          <t>10:49:10</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1994,7 +1994,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Tue, 07 Mar 2023</t>
+          <t>Mon, 13 Mar 2023</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -2014,7 +2014,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>10:45:02</t>
+          <t>10:49:10</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -2420,7 +2420,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Tue, 07 Mar 2023</t>
+          <t>Mon, 13 Mar 2023</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -2440,7 +2440,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>10:45:02</t>
+          <t>10:49:10</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -2767,7 +2767,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Tue, 07 Mar 2023</t>
+          <t>Mon, 13 Mar 2023</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -2787,7 +2787,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>10:45:02</t>
+          <t>10:49:10</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">

</xml_diff>

<commit_message>
adding timestamps to output names
</commit_message>
<xml_diff>
--- a/notebooks/test_results.xlsx
+++ b/notebooks/test_results.xlsx
@@ -8,13 +8,15 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="description" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_0" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_2" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_3" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_5" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_6" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_7" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_8" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_0_(2023-03-20-09-47-09-86)" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_1_(2023-03-20-09-47-09-93)" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_2_(2023-03-20-09-47-10-00)" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_3_(2023-03-20-09-47-10-07)" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_4_(2023-03-20-09-47-10-15)" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_5_(2023-03-20-09-47-10-21)" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_6_(2023-03-20-09-47-10-27)" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_7_(2023-03-20-09-47-10-34)" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="output_8_(2023-03-20-09-47-10-42)" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -432,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,7 +462,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>output_0</t>
+          <t>output_0_(2023-03-20-09-47-09-86)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -477,103 +479,484 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>output_2</t>
+          <t>output_1_(2023-03-20-09-47-09-93)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>safe_table = acro.crosstab(df.year, df.grant_type, values=negative, aggfunc="mean")</t>
+          <t>safe_table = acro.crosstab(df.year, df.grant_type, values=df.inc_grants, aggfunc="mean")</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>review; negative values found</t>
+          <t xml:space="preserve">fail; threshold: 6 cells suppressed; p-ratio: 1 cells suppressed; nk-rule: 1 cells suppressed; </t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>output_3</t>
+          <t>output_2_(2023-03-20-09-47-10-00)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>table = acro.pivot_table(</t>
+          <t>safe_table = acro.crosstab(df.year, df.grant_type, values=negative, aggfunc="mean")</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>pass</t>
+          <t>review; negative values found</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>output_5</t>
+          <t>output_3_(2023-03-20-09-47-10-07)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>results = acro.ols(y, x)</t>
+          <t>table = acro.pivot_table(</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>pass; dof=807.0 &gt;= 10</t>
+          <t>pass</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>output_6</t>
+          <t>output_4_(2023-03-20-09-47-10-15)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>results = acro.olsr(</t>
+          <t>table = acro.pivot_table(</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>pass; dof=807.0 &gt;= 10</t>
+          <t>review; negative values found</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>output_7</t>
+          <t>output_5_(2023-03-20-09-47-10-21)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>results = acro.probit(y, x)</t>
+          <t>results = acro.ols(y, x)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>pass; dof=806.0 &gt;= 10</t>
+          <t>pass; dof=807.0 &gt;= 10</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>output_8</t>
+          <t>output_6_(2023-03-20-09-47-10-27)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>results = acro.olsr(</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>pass; dof=807.0 &gt;= 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>output_7_(2023-03-20-09-47-10-34)</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>results = acro.probit(y, x)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>pass; dof=806.0 &gt;= 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>output_8_(2023-03-20-09-47-10-42)</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>results = acro.logit(y, x)</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>pass; dof=806.0 &gt;= 10</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Command</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>results = acro.logit(y, x)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Summary</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>pass; dof=806.0 &gt;= 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Dep. Variable:</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>survivor</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>No. Observations:</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>811</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Model:</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Logit</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Df Residuals:</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Method:</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>MLE</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Df Model:</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Date:</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Mon, 20 Mar 2023</t>
+        </is>
+      </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>pass; dof=806.0 &gt;= 10</t>
-        </is>
+          <t>Pseudo R-squ.:</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.2187</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Time:</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>09:47:10</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Log-Likelihood:</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>-398.07</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>converged:</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>LL-Null:</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>-509.5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Covariance Type:</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>nonrobust</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>LLR p-value:</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>4.532e-47</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>coef</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>std err</t>
+        </is>
+      </c>
+      <c r="D13" s="1" t="inlineStr">
+        <is>
+          <t>z</t>
+        </is>
+      </c>
+      <c r="E13" s="1" t="inlineStr">
+        <is>
+          <t>P&gt;|z|</t>
+        </is>
+      </c>
+      <c r="F13" s="1" t="inlineStr">
+        <is>
+          <t>[0.025</t>
+        </is>
+      </c>
+      <c r="G13" s="1" t="inlineStr">
+        <is>
+          <t>0.975]</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>const</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.0512</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.091</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.5610000000000001</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-0.128</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>inc_activity</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>2.981e-07</v>
+      </c>
+      <c r="C15" t="n">
+        <v>8.95e-08</v>
+      </c>
+      <c r="D15" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1.23e-07</v>
+      </c>
+      <c r="G15" t="n">
+        <v>4.74e-07</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>inc_grants</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1.351e-07</v>
+      </c>
+      <c r="C16" t="n">
+        <v>6.67e-08</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2.026</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="F16" t="n">
+        <v>4.39e-09</v>
+      </c>
+      <c r="G16" t="n">
+        <v>2.66e-07</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>inc_donations</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>5.122999999999999e-07</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1.04e-07</v>
+      </c>
+      <c r="D17" t="n">
+        <v>4.927</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>3.08e-07</v>
+      </c>
+      <c r="G17" t="n">
+        <v>7.16e-07</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>total_costs</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>-1.442e-07</v>
+      </c>
+      <c r="C18" t="n">
+        <v>6.26e-08</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-2.304</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.021</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-2.67e-07</v>
+      </c>
+      <c r="G18" t="n">
+        <v>-2.15e-08</v>
       </c>
     </row>
   </sheetData>
@@ -950,7 +1333,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>safe_table = acro.crosstab(df.year, df.grant_type, values=negative, aggfunc="mean")</t>
+          <t>safe_table = acro.crosstab(df.year, df.grant_type, values=df.inc_grants, aggfunc="mean")</t>
         </is>
       </c>
     </row>
@@ -962,7 +1345,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>review; negative values found</t>
+          <t xml:space="preserve">fail; threshold: 6 cells suppressed; p-ratio: 1 cells suppressed; nk-rule: 1 cells suppressed; </t>
         </is>
       </c>
     </row>
@@ -997,95 +1380,151 @@
       <c r="A6" s="1" t="n">
         <v>2010</v>
       </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>negative</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">threshold; p-ratio; nk-rule; </t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>2011</v>
       </c>
-      <c r="B7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>ok</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>negative</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">threshold; </t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
         <v>2012</v>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>negative</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">threshold; </t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>2013</v>
       </c>
-      <c r="B9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>ok</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>negative</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">threshold; </t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
         <v>2014</v>
       </c>
-      <c r="B10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>ok</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>negative</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr"/>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">threshold; </t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
         <v>2015</v>
       </c>
-      <c r="B11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>ok</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>negative</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">threshold; </t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -1125,11 +1564,9 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>8280032.5</v>
-      </c>
-      <c r="E14" t="n">
-        <v>11636000</v>
-      </c>
+        <v>8402284</v>
+      </c>
+      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1139,14 +1576,12 @@
         <v>8502247</v>
       </c>
       <c r="C15" t="n">
-        <v>123496.4453125</v>
+        <v>124013.859375</v>
       </c>
       <c r="D15" t="n">
-        <v>7577703.5</v>
-      </c>
-      <c r="E15" t="n">
-        <v>16047500</v>
-      </c>
+        <v>7716880</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1159,11 +1594,9 @@
         <v>131859.0625</v>
       </c>
       <c r="D16" t="n">
-        <v>6796357.5</v>
-      </c>
-      <c r="E16" t="n">
-        <v>16810000</v>
-      </c>
+        <v>6958050.5</v>
+      </c>
+      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1173,14 +1606,12 @@
         <v>13557147</v>
       </c>
       <c r="C17" t="n">
-        <v>147937.625</v>
+        <v>147937.796875</v>
       </c>
       <c r="D17" t="n">
-        <v>6988263.5</v>
-      </c>
-      <c r="E17" t="n">
-        <v>16765625</v>
-      </c>
+        <v>7202273.5</v>
+      </c>
+      <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1190,14 +1621,12 @@
         <v>13748147</v>
       </c>
       <c r="C18" t="n">
-        <v>133198.078125</v>
+        <v>133198.25</v>
       </c>
       <c r="D18" t="n">
-        <v>7997392.5</v>
-      </c>
-      <c r="E18" t="n">
-        <v>17845750</v>
-      </c>
+        <v>8277525.5</v>
+      </c>
+      <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1207,14 +1636,12 @@
         <v>11133433</v>
       </c>
       <c r="C19" t="n">
-        <v>146572.015625</v>
+        <v>146572.1875</v>
       </c>
       <c r="D19" t="n">
-        <v>10388613</v>
-      </c>
-      <c r="E19" t="n">
-        <v>18278624</v>
-      </c>
+        <v>10812888</v>
+      </c>
+      <c r="E19" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1222,6 +1649,304 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Command</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>safe_table = acro.crosstab(df.year, df.grant_type, values=negative, aggfunc="mean")</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Summary</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>review; negative values found</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>R/G</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="D13" s="1" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="E13" s="1" t="inlineStr">
+        <is>
+          <t>R/G</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B14" t="n">
+        <v>9921906</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>8280032.5</v>
+      </c>
+      <c r="E14" t="n">
+        <v>11636000</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B15" t="n">
+        <v>8502247</v>
+      </c>
+      <c r="C15" t="n">
+        <v>123496.4453125</v>
+      </c>
+      <c r="D15" t="n">
+        <v>7577703.5</v>
+      </c>
+      <c r="E15" t="n">
+        <v>16047500</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B16" t="n">
+        <v>11458580</v>
+      </c>
+      <c r="C16" t="n">
+        <v>131859.0625</v>
+      </c>
+      <c r="D16" t="n">
+        <v>6796357.5</v>
+      </c>
+      <c r="E16" t="n">
+        <v>16810000</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B17" t="n">
+        <v>13557147</v>
+      </c>
+      <c r="C17" t="n">
+        <v>147937.625</v>
+      </c>
+      <c r="D17" t="n">
+        <v>6988263.5</v>
+      </c>
+      <c r="E17" t="n">
+        <v>16765625</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B18" t="n">
+        <v>13748147</v>
+      </c>
+      <c r="C18" t="n">
+        <v>133198.078125</v>
+      </c>
+      <c r="D18" t="n">
+        <v>7997392.5</v>
+      </c>
+      <c r="E18" t="n">
+        <v>17845750</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B19" t="n">
+        <v>11133433</v>
+      </c>
+      <c r="C19" t="n">
+        <v>146572.015625</v>
+      </c>
+      <c r="D19" t="n">
+        <v>10388613</v>
+      </c>
+      <c r="E19" t="n">
+        <v>18278624</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1455,7 +2180,225 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Command</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>table = acro.pivot_table(</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Summary</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>review; negative values found</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr"/>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>std</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr"/>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>inc_grants</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>inc_grants</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>grant_type</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>R/G</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr"/>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>std</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr"/>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>inc_grants</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>inc_grants</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>grant_type</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>11412787</v>
+      </c>
+      <c r="C16" t="n">
+        <v>22832202.73499117</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>134180.046875</v>
+      </c>
+      <c r="C17" t="n">
+        <v>199019.5648370635</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>7882231</v>
+      </c>
+      <c r="C18" t="n">
+        <v>32045584.8569128</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>R/G</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>16648273</v>
+      </c>
+      <c r="C19" t="n">
+        <v>15835323.99322482</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1568,7 +2511,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Mon, 13 Mar 2023</t>
+          <t>Mon, 20 Mar 2023</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1588,7 +2531,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>10:49:10</t>
+          <t>09:47:10</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1881,7 +2824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1994,7 +2937,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Mon, 13 Mar 2023</t>
+          <t>Mon, 20 Mar 2023</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -2014,7 +2957,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>10:49:10</t>
+          <t>09:47:10</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -2307,7 +3250,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2420,7 +3363,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Mon, 13 Mar 2023</t>
+          <t>Mon, 20 Mar 2023</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -2440,7 +3383,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>10:49:10</t>
+          <t>09:47:10</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -2647,353 +3590,6 @@
       </c>
       <c r="G18" t="n">
         <v>-1.44e-08</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Command</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>results = acro.logit(y, x)</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Summary</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>pass; dof=806.0 &gt;= 10</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Dep. Variable:</t>
-        </is>
-      </c>
-      <c r="B5" s="1" t="inlineStr">
-        <is>
-          <t>survivor</t>
-        </is>
-      </c>
-      <c r="C5" s="1" t="inlineStr">
-        <is>
-          <t>No. Observations:</t>
-        </is>
-      </c>
-      <c r="D5" s="1" t="inlineStr">
-        <is>
-          <t>811</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Model:</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Logit</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Df Residuals:</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Method:</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>MLE</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Df Model:</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Date:</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Mon, 13 Mar 2023</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Pseudo R-squ.:</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>0.2187</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>Time:</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>10:49:10</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Log-Likelihood:</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>-398.07</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>converged:</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>LL-Null:</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>-509.5</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>Covariance Type:</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>nonrobust</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>LLR p-value:</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>4.532e-47</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" s="1" t="inlineStr">
-        <is>
-          <t>coef</t>
-        </is>
-      </c>
-      <c r="C13" s="1" t="inlineStr">
-        <is>
-          <t>std err</t>
-        </is>
-      </c>
-      <c r="D13" s="1" t="inlineStr">
-        <is>
-          <t>z</t>
-        </is>
-      </c>
-      <c r="E13" s="1" t="inlineStr">
-        <is>
-          <t>P&gt;|z|</t>
-        </is>
-      </c>
-      <c r="F13" s="1" t="inlineStr">
-        <is>
-          <t>[0.025</t>
-        </is>
-      </c>
-      <c r="G13" s="1" t="inlineStr">
-        <is>
-          <t>0.975]</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>const</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>0.0512</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.091</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.5610000000000001</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.575</v>
-      </c>
-      <c r="F14" t="n">
-        <v>-0.128</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.23</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>inc_activity</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>2.981e-07</v>
-      </c>
-      <c r="C15" t="n">
-        <v>8.95e-08</v>
-      </c>
-      <c r="D15" t="n">
-        <v>3.33</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="F15" t="n">
-        <v>1.23e-07</v>
-      </c>
-      <c r="G15" t="n">
-        <v>4.74e-07</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>inc_grants</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>1.351e-07</v>
-      </c>
-      <c r="C16" t="n">
-        <v>6.67e-08</v>
-      </c>
-      <c r="D16" t="n">
-        <v>2.026</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.043</v>
-      </c>
-      <c r="F16" t="n">
-        <v>4.39e-09</v>
-      </c>
-      <c r="G16" t="n">
-        <v>2.66e-07</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>inc_donations</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>5.122999999999999e-07</v>
-      </c>
-      <c r="C17" t="n">
-        <v>1.04e-07</v>
-      </c>
-      <c r="D17" t="n">
-        <v>4.927</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" t="n">
-        <v>3.08e-07</v>
-      </c>
-      <c r="G17" t="n">
-        <v>7.16e-07</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>total_costs</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>-1.442e-07</v>
-      </c>
-      <c r="C18" t="n">
-        <v>6.26e-08</v>
-      </c>
-      <c r="D18" t="n">
-        <v>-2.304</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.021</v>
-      </c>
-      <c r="F18" t="n">
-        <v>-2.67e-07</v>
-      </c>
-      <c r="G18" t="n">
-        <v>-2.15e-08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>